<commit_message>
HTB beats AIP with a royal flush
</commit_message>
<xml_diff>
--- a/4004-F18-A2-correctionGrid.xlsx
+++ b/4004-F18-A2-correctionGrid.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thinkpad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thinkpad\Documents\GitHub\comp4004-A2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CB554F-E8B1-423D-9D58-D7381AB84216}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FD488F-F122-4B23-A668-849B40002C40}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="177">
   <si>
     <t>First Name</t>
   </si>
@@ -571,6 +571,12 @@
   </si>
   <si>
     <t>IsItAPair.java</t>
+  </si>
+  <si>
+    <t>HTB_royal_flush_beats_AIP.feature</t>
+  </si>
+  <si>
+    <t>HTBRoyalFlushBeatsAIP.java</t>
   </si>
 </sst>
 </file>
@@ -2112,8 +2118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2560,14 +2566,18 @@
         <v>26</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="12">
         <v>0.5</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
+      <c r="E19" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>176</v>
+      </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="20"/>
@@ -2586,14 +2596,18 @@
         <v>27</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="12">
         <v>0.5</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="E20" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>176</v>
+      </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="20"/>
@@ -2612,14 +2626,18 @@
         <v>28</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="12">
         <v>0.5</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
+      <c r="E21" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>176</v>
+      </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -2635,14 +2653,18 @@
         <v>29</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="12">
         <v>0.5</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
+      <c r="E22" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>176</v>
+      </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -2658,14 +2680,18 @@
         <v>30</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="12">
         <v>0.5</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="E23" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>176</v>
+      </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -2681,14 +2707,18 @@
         <v>31</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="12">
         <v>0.5</v>
       </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
+      <c r="E24" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>176</v>
+      </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -2704,14 +2734,18 @@
         <v>32</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="12">
         <v>0.5</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="E25" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>176</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -2727,14 +2761,18 @@
         <v>33</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="12">
         <v>0.5</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="E26" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>176</v>
+      </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -2750,14 +2788,18 @@
         <v>34</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="12">
         <v>0.5</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="E27" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>176</v>
+      </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>

</xml_diff>

<commit_message>
Added HTB beats AIP tests
</commit_message>
<xml_diff>
--- a/4004-F18-A2-correctionGrid.xlsx
+++ b/4004-F18-A2-correctionGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thinkpad\Documents\GitHub\comp4004-A2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FD488F-F122-4B23-A668-849B40002C40}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5EE935-FA18-403D-A5EE-901575B37125}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="193">
   <si>
     <t>First Name</t>
   </si>
@@ -577,6 +577,54 @@
   </si>
   <si>
     <t>HTBRoyalFlushBeatsAIP.java</t>
+  </si>
+  <si>
+    <t>HTB_straight_flush_beats_AIP.feature</t>
+  </si>
+  <si>
+    <t>HTBStraightFlushBeatsAIP.java</t>
+  </si>
+  <si>
+    <t>HTB_four_of_a_kind_beats_AIP.feature</t>
+  </si>
+  <si>
+    <t>HTBFourOfAKindBeatsAIP.java</t>
+  </si>
+  <si>
+    <t>HTB_full_house_beats_AIP.feature</t>
+  </si>
+  <si>
+    <t>HTBFullHouseBeatsAIP.java</t>
+  </si>
+  <si>
+    <t>HTB_flush_beats_AIP.feature</t>
+  </si>
+  <si>
+    <t>HTBFlushBeatsAIP.java</t>
+  </si>
+  <si>
+    <t>HTB_straight_beats_AIP.feature</t>
+  </si>
+  <si>
+    <t>HTBStraightBeatsAIP.java</t>
+  </si>
+  <si>
+    <t>HTB_three_of_a_kind_beats_AIP.feature</t>
+  </si>
+  <si>
+    <t>HTBThreeOfAKindBeatsAIP.java</t>
+  </si>
+  <si>
+    <t>HTB_two_pair_beats_AIP.feature</t>
+  </si>
+  <si>
+    <t>HTBTwoPairBeatsAIP.java</t>
+  </si>
+  <si>
+    <t>HTB_pair_beats_AIP.feature</t>
+  </si>
+  <si>
+    <t>HTBPairBeatsAIP.java</t>
   </si>
 </sst>
 </file>
@@ -2118,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2815,14 +2863,18 @@
         <v>35</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="12">
         <v>0.5</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="E28" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>178</v>
+      </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -2838,14 +2890,18 @@
         <v>36</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="12">
         <v>0.5</v>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+      <c r="E29" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>178</v>
+      </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2861,14 +2917,18 @@
         <v>37</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="12">
         <v>0.5</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="E30" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>178</v>
+      </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -2884,14 +2944,18 @@
         <v>38</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="12">
         <v>0.5</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
+      <c r="E31" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>178</v>
+      </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
@@ -2906,14 +2970,18 @@
         <v>39</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="12">
         <v>0.5</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
+      <c r="E32" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>178</v>
+      </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
@@ -2929,14 +2997,18 @@
         <v>40</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C33" s="23"/>
       <c r="D33" s="12">
         <v>0.5</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
+      <c r="E33" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>178</v>
+      </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -2952,14 +3024,18 @@
         <v>41</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C34" s="23"/>
       <c r="D34" s="12">
         <v>0.5</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
+      <c r="E34" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>178</v>
+      </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
@@ -2975,14 +3051,18 @@
         <v>42</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="12">
         <v>0.5</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
+      <c r="E35" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>178</v>
+      </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2998,14 +3078,18 @@
         <v>44</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="12">
         <v>0.5</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
+      <c r="E36" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>180</v>
+      </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -3021,14 +3105,18 @@
         <v>45</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="12">
         <v>0.5</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
+      <c r="E37" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>180</v>
+      </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
@@ -3044,14 +3132,18 @@
         <v>46</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C38" s="23"/>
       <c r="D38" s="12">
         <v>0.5</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
+      <c r="E38" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>180</v>
+      </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
@@ -3067,14 +3159,18 @@
         <v>47</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="12">
         <v>0.5</v>
       </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
+      <c r="E39" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>180</v>
+      </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -3090,14 +3186,18 @@
         <v>48</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C40" s="23"/>
       <c r="D40" s="12">
         <v>0.5</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
+      <c r="E40" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>180</v>
+      </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -3113,14 +3213,18 @@
         <v>49</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="12">
         <v>0.5</v>
       </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
+      <c r="E41" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>180</v>
+      </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
@@ -3136,14 +3240,18 @@
         <v>50</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C42" s="23"/>
       <c r="D42" s="12">
         <v>0.5</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
+      <c r="E42" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>180</v>
+      </c>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
@@ -3158,14 +3266,18 @@
         <v>51</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="12">
         <v>0.5</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
+      <c r="E43" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>182</v>
+      </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
@@ -3180,14 +3292,18 @@
         <v>52</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="12">
         <v>0.5</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
+      <c r="E44" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>182</v>
+      </c>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
@@ -3202,14 +3318,18 @@
         <v>53</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="12">
         <v>0.5</v>
       </c>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
+      <c r="E45" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>182</v>
+      </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
@@ -3224,14 +3344,18 @@
         <v>54</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="12">
         <v>0.5</v>
       </c>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
+      <c r="E46" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>182</v>
+      </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
@@ -3246,14 +3370,18 @@
         <v>55</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="12">
         <v>0.5</v>
       </c>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
+      <c r="E47" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>182</v>
+      </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
@@ -3268,14 +3396,18 @@
         <v>56</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="12">
         <v>0.5</v>
       </c>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
+      <c r="E48" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F48" s="29" t="s">
+        <v>182</v>
+      </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
@@ -3290,14 +3422,18 @@
         <v>57</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="12">
         <v>0.5</v>
       </c>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
+      <c r="E49" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="F49" s="29" t="s">
+        <v>184</v>
+      </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
@@ -3312,14 +3448,18 @@
         <v>58</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="12">
         <v>0.5</v>
       </c>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
+      <c r="E50" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="F50" s="29" t="s">
+        <v>184</v>
+      </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -3334,14 +3474,18 @@
         <v>59</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51" s="12">
         <v>0.5</v>
       </c>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
+      <c r="E51" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="F51" s="29" t="s">
+        <v>184</v>
+      </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
@@ -3356,14 +3500,18 @@
         <v>60</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C52" s="23"/>
       <c r="D52" s="12">
         <v>0.5</v>
       </c>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
+      <c r="E52" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>184</v>
+      </c>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
@@ -3378,14 +3526,18 @@
         <v>61</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C53" s="23"/>
       <c r="D53" s="12">
         <v>0.5</v>
       </c>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
+      <c r="E53" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="F53" s="29" t="s">
+        <v>184</v>
+      </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
@@ -3400,14 +3552,18 @@
         <v>62</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C54" s="23"/>
       <c r="D54" s="12">
         <v>0.5</v>
       </c>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
+      <c r="E54" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F54" s="29" t="s">
+        <v>186</v>
+      </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
@@ -3422,14 +3578,18 @@
         <v>63</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C55" s="23"/>
       <c r="D55" s="12">
         <v>0.5</v>
       </c>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
+      <c r="E55" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F55" s="29" t="s">
+        <v>186</v>
+      </c>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
@@ -3444,14 +3604,18 @@
         <v>64</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C56" s="23"/>
       <c r="D56" s="12">
         <v>0.5</v>
       </c>
-      <c r="E56" s="29"/>
-      <c r="F56" s="29"/>
+      <c r="E56" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F56" s="29" t="s">
+        <v>186</v>
+      </c>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
@@ -3466,14 +3630,18 @@
         <v>65</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C57" s="23"/>
       <c r="D57" s="12">
         <v>0.5</v>
       </c>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29"/>
+      <c r="E57" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F57" s="29" t="s">
+        <v>186</v>
+      </c>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
@@ -3488,14 +3656,18 @@
         <v>66</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C58" s="23"/>
       <c r="D58" s="12">
         <v>0.5</v>
       </c>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
+      <c r="E58" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="F58" s="29" t="s">
+        <v>188</v>
+      </c>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
@@ -3510,14 +3682,18 @@
         <v>67</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C59" s="23"/>
       <c r="D59" s="12">
         <v>0.5</v>
       </c>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
+      <c r="E59" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="F59" s="29" t="s">
+        <v>188</v>
+      </c>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
@@ -3532,14 +3708,18 @@
         <v>68</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C60" s="23"/>
       <c r="D60" s="12">
         <v>0.5</v>
       </c>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
+      <c r="E60" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="F60" s="29" t="s">
+        <v>188</v>
+      </c>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
@@ -3554,14 +3734,18 @@
         <v>69</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C61" s="23"/>
       <c r="D61" s="12">
         <v>0.5</v>
       </c>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
+      <c r="E61" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="F61" s="29" t="s">
+        <v>190</v>
+      </c>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
@@ -3576,14 +3760,18 @@
         <v>70</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C62" s="23"/>
       <c r="D62" s="12">
         <v>0.5</v>
       </c>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
+      <c r="E62" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="F62" s="29" t="s">
+        <v>190</v>
+      </c>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
@@ -3598,14 +3786,18 @@
         <v>71</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C63" s="23"/>
       <c r="D63" s="12">
         <v>0.5</v>
       </c>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
+      <c r="E63" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="F63" s="29" t="s">
+        <v>192</v>
+      </c>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>

</xml_diff>

<commit_message>
Added AIP beats HTB tests
</commit_message>
<xml_diff>
--- a/4004-F18-A2-correctionGrid.xlsx
+++ b/4004-F18-A2-correctionGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thinkpad\Documents\GitHub\comp4004-A2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5EE935-FA18-403D-A5EE-901575B37125}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC2FB5-AA6C-4E3D-82AB-6EFD1841334C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="207">
   <si>
     <t>First Name</t>
   </si>
@@ -625,6 +625,48 @@
   </si>
   <si>
     <t>HTBPairBeatsAIP.java</t>
+  </si>
+  <si>
+    <t>AIP_royal_flush_beats_HTB.feature</t>
+  </si>
+  <si>
+    <t>AIPRoyalFlushBeatsHTB.java</t>
+  </si>
+  <si>
+    <t>AIP_straight_flush_beats_HTB.feature</t>
+  </si>
+  <si>
+    <t>AIPStraightFlushBeatsHTB.java</t>
+  </si>
+  <si>
+    <t>AIP_four_of_a_kind_beats_HTB.feature</t>
+  </si>
+  <si>
+    <t>AIPFourOfAKindBeatsHTB.java</t>
+  </si>
+  <si>
+    <t>AIP_full_house_beats_HTB.feature</t>
+  </si>
+  <si>
+    <t>AIPFullHouseBeatsHTB.java</t>
+  </si>
+  <si>
+    <t>AIP_flush_beats_HTB.feature</t>
+  </si>
+  <si>
+    <t>AIPFlushBeatsHTB.java</t>
+  </si>
+  <si>
+    <t>AIP_straight_beats_HTB.feature</t>
+  </si>
+  <si>
+    <t>AIPStraightBeatsHTB.java</t>
+  </si>
+  <si>
+    <t>feature file</t>
+  </si>
+  <si>
+    <t>java file</t>
   </si>
 </sst>
 </file>
@@ -2166,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A100" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2314,8 +2356,12 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>206</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -3828,14 +3874,18 @@
         <v>72</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C65" s="23"/>
       <c r="D65" s="12">
         <v>0.5</v>
       </c>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
+      <c r="E65" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>194</v>
+      </c>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
@@ -3850,14 +3900,18 @@
         <v>73</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C66" s="23"/>
       <c r="D66" s="12">
         <v>0.5</v>
       </c>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
+      <c r="E66" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>194</v>
+      </c>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
@@ -3872,14 +3926,18 @@
         <v>74</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C67" s="23"/>
       <c r="D67" s="12">
         <v>0.5</v>
       </c>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
+      <c r="E67" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>194</v>
+      </c>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
@@ -3894,14 +3952,18 @@
         <v>75</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C68" s="23"/>
       <c r="D68" s="12">
         <v>0.5</v>
       </c>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
+      <c r="E68" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>194</v>
+      </c>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
@@ -3918,14 +3980,18 @@
         <v>76</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C69" s="23"/>
       <c r="D69" s="12">
         <v>0.5</v>
       </c>
-      <c r="E69" s="29"/>
-      <c r="F69" s="29"/>
+      <c r="E69" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>194</v>
+      </c>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
@@ -3942,14 +4008,18 @@
         <v>77</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C70" s="23"/>
       <c r="D70" s="12">
         <v>0.5</v>
       </c>
-      <c r="E70" s="29"/>
-      <c r="F70" s="29"/>
+      <c r="E70" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F70" s="29" t="s">
+        <v>194</v>
+      </c>
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
@@ -3966,14 +4036,18 @@
         <v>78</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C71" s="23"/>
       <c r="D71" s="12">
         <v>0.5</v>
       </c>
-      <c r="E71" s="29"/>
-      <c r="F71" s="29"/>
+      <c r="E71" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F71" s="29" t="s">
+        <v>194</v>
+      </c>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
@@ -3990,14 +4064,18 @@
         <v>79</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C72" s="23"/>
       <c r="D72" s="12">
         <v>0.5</v>
       </c>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
+      <c r="E72" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F72" s="29" t="s">
+        <v>194</v>
+      </c>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
@@ -4014,14 +4092,18 @@
         <v>80</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C73" s="23"/>
       <c r="D73" s="12">
         <v>0.5</v>
       </c>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
+      <c r="E73" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F73" s="29" t="s">
+        <v>194</v>
+      </c>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
@@ -4038,14 +4120,18 @@
         <v>81</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C74" s="23"/>
       <c r="D74" s="12">
         <v>0.5</v>
       </c>
-      <c r="E74" s="29"/>
-      <c r="F74" s="29"/>
+      <c r="E74" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F74" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
@@ -4062,14 +4148,18 @@
         <v>82</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C75" s="23"/>
       <c r="D75" s="12">
         <v>0.5</v>
       </c>
-      <c r="E75" s="29"/>
-      <c r="F75" s="29"/>
+      <c r="E75" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F75" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
@@ -4086,14 +4176,18 @@
         <v>83</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C76" s="23"/>
       <c r="D76" s="12">
         <v>0.5</v>
       </c>
-      <c r="E76" s="29"/>
-      <c r="F76" s="29"/>
+      <c r="E76" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F76" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
@@ -4110,14 +4204,18 @@
         <v>84</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C77" s="23"/>
       <c r="D77" s="12">
         <v>0.5</v>
       </c>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
+      <c r="E77" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F77" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
@@ -4134,14 +4232,18 @@
         <v>85</v>
       </c>
       <c r="B78" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C78" s="23"/>
       <c r="D78" s="12">
         <v>0.5</v>
       </c>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
+      <c r="E78" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F78" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
@@ -4158,14 +4260,18 @@
         <v>86</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C79" s="23"/>
       <c r="D79" s="12">
         <v>0.5</v>
       </c>
-      <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
+      <c r="E79" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F79" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
@@ -4182,14 +4288,18 @@
         <v>87</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C80" s="23"/>
       <c r="D80" s="12">
         <v>0.5</v>
       </c>
-      <c r="E80" s="29"/>
-      <c r="F80" s="29"/>
+      <c r="E80" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F80" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
@@ -4206,14 +4316,18 @@
         <v>88</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="12">
         <v>0.5</v>
       </c>
-      <c r="E81" s="29"/>
-      <c r="F81" s="29"/>
+      <c r="E81" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F81" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
@@ -4230,14 +4344,18 @@
         <v>89</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C82" s="23"/>
       <c r="D82" s="12">
         <v>0.5</v>
       </c>
-      <c r="E82" s="29"/>
-      <c r="F82" s="29"/>
+      <c r="E82" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F82" s="29" t="s">
+        <v>198</v>
+      </c>
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
@@ -4254,14 +4372,18 @@
         <v>90</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C83" s="23"/>
       <c r="D83" s="12">
         <v>0.5</v>
       </c>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
+      <c r="E83" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F83" s="29" t="s">
+        <v>198</v>
+      </c>
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
@@ -4278,14 +4400,18 @@
         <v>91</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C84" s="23"/>
       <c r="D84" s="12">
         <v>0.5</v>
       </c>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
+      <c r="E84" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F84" s="29" t="s">
+        <v>198</v>
+      </c>
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
@@ -4303,14 +4429,18 @@
         <v>92</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C85" s="23"/>
       <c r="D85" s="12">
         <v>0.5</v>
       </c>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
+      <c r="E85" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F85" s="29" t="s">
+        <v>198</v>
+      </c>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
@@ -4328,14 +4458,18 @@
         <v>94</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C86" s="23"/>
       <c r="D86" s="12">
         <v>0.5</v>
       </c>
-      <c r="E86" s="29"/>
-      <c r="F86" s="29"/>
+      <c r="E86" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F86" s="29" t="s">
+        <v>198</v>
+      </c>
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
@@ -4353,14 +4487,18 @@
         <v>95</v>
       </c>
       <c r="B87" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C87" s="23"/>
       <c r="D87" s="12">
         <v>0.5</v>
       </c>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
+      <c r="E87" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F87" s="29" t="s">
+        <v>198</v>
+      </c>
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
@@ -4378,14 +4516,18 @@
         <v>93</v>
       </c>
       <c r="B88" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C88" s="23"/>
       <c r="D88" s="12">
         <v>0.5</v>
       </c>
-      <c r="E88" s="29"/>
-      <c r="F88" s="29"/>
+      <c r="E88" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F88" s="29" t="s">
+        <v>198</v>
+      </c>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
@@ -4403,14 +4545,18 @@
         <v>96</v>
       </c>
       <c r="B89" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C89" s="23"/>
       <c r="D89" s="12">
         <v>0.5</v>
       </c>
-      <c r="E89" s="29"/>
-      <c r="F89" s="29"/>
+      <c r="E89" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="F89" s="29" t="s">
+        <v>200</v>
+      </c>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
@@ -4428,14 +4574,18 @@
         <v>97</v>
       </c>
       <c r="B90" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C90" s="23"/>
       <c r="D90" s="12">
         <v>0.5</v>
       </c>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
+      <c r="E90" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="F90" s="29" t="s">
+        <v>200</v>
+      </c>
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
@@ -4452,14 +4602,18 @@
         <v>98</v>
       </c>
       <c r="B91" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C91" s="23"/>
       <c r="D91" s="12">
         <v>0.5</v>
       </c>
-      <c r="E91" s="29"/>
-      <c r="F91" s="29"/>
+      <c r="E91" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="F91" s="29" t="s">
+        <v>200</v>
+      </c>
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
@@ -4476,14 +4630,18 @@
         <v>99</v>
       </c>
       <c r="B92" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C92" s="23"/>
       <c r="D92" s="12">
         <v>0.5</v>
       </c>
-      <c r="E92" s="29"/>
-      <c r="F92" s="29"/>
+      <c r="E92" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="F92" s="29" t="s">
+        <v>200</v>
+      </c>
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
@@ -4500,14 +4658,18 @@
         <v>100</v>
       </c>
       <c r="B93" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C93" s="23"/>
       <c r="D93" s="12">
         <v>0.5</v>
       </c>
-      <c r="E93" s="29"/>
-      <c r="F93" s="29"/>
+      <c r="E93" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="F93" s="29" t="s">
+        <v>200</v>
+      </c>
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
@@ -4524,14 +4686,18 @@
         <v>101</v>
       </c>
       <c r="B94" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C94" s="23"/>
       <c r="D94" s="12">
         <v>0.5</v>
       </c>
-      <c r="E94" s="29"/>
-      <c r="F94" s="29"/>
+      <c r="E94" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="F94" s="29" t="s">
+        <v>200</v>
+      </c>
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
@@ -4548,14 +4714,18 @@
         <v>102</v>
       </c>
       <c r="B95" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C95" s="23"/>
       <c r="D95" s="12">
         <v>0.5</v>
       </c>
-      <c r="E95" s="29"/>
-      <c r="F95" s="29"/>
+      <c r="E95" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F95" s="29" t="s">
+        <v>202</v>
+      </c>
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
@@ -4572,14 +4742,18 @@
         <v>103</v>
       </c>
       <c r="B96" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C96" s="23"/>
       <c r="D96" s="12">
         <v>0.5</v>
       </c>
-      <c r="E96" s="29"/>
-      <c r="F96" s="29"/>
+      <c r="E96" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F96" s="29" t="s">
+        <v>202</v>
+      </c>
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
@@ -4596,14 +4770,18 @@
         <v>104</v>
       </c>
       <c r="B97" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C97" s="23"/>
       <c r="D97" s="12">
         <v>0.5</v>
       </c>
-      <c r="E97" s="29"/>
-      <c r="F97" s="29"/>
+      <c r="E97" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F97" s="29" t="s">
+        <v>202</v>
+      </c>
       <c r="G97" s="7"/>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
@@ -4620,14 +4798,18 @@
         <v>105</v>
       </c>
       <c r="B98" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C98" s="23"/>
       <c r="D98" s="12">
         <v>0.5</v>
       </c>
-      <c r="E98" s="29"/>
-      <c r="F98" s="29"/>
+      <c r="E98" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F98" s="29" t="s">
+        <v>202</v>
+      </c>
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
@@ -4644,14 +4826,18 @@
         <v>106</v>
       </c>
       <c r="B99" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C99" s="23"/>
       <c r="D99" s="12">
         <v>0.5</v>
       </c>
-      <c r="E99" s="29"/>
-      <c r="F99" s="29"/>
+      <c r="E99" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F99" s="29" t="s">
+        <v>202</v>
+      </c>
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
@@ -4668,14 +4854,18 @@
         <v>107</v>
       </c>
       <c r="B100" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C100" s="23"/>
       <c r="D100" s="12">
         <v>0.5</v>
       </c>
-      <c r="E100" s="29"/>
-      <c r="F100" s="29"/>
+      <c r="E100" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F100" s="29" t="s">
+        <v>204</v>
+      </c>
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
@@ -4692,14 +4882,18 @@
         <v>108</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C101" s="23"/>
       <c r="D101" s="12">
         <v>0.5</v>
       </c>
-      <c r="E101" s="29"/>
-      <c r="F101" s="29"/>
+      <c r="E101" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F101" s="29" t="s">
+        <v>204</v>
+      </c>
       <c r="G101" s="7"/>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
@@ -4716,14 +4910,18 @@
         <v>109</v>
       </c>
       <c r="B102" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C102" s="23"/>
       <c r="D102" s="12">
         <v>0.5</v>
       </c>
-      <c r="E102" s="29"/>
-      <c r="F102" s="29"/>
+      <c r="E102" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F102" s="29" t="s">
+        <v>204</v>
+      </c>
       <c r="G102" s="7"/>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
@@ -4740,14 +4938,18 @@
         <v>110</v>
       </c>
       <c r="B103" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C103" s="23"/>
       <c r="D103" s="12">
         <v>0.5</v>
       </c>
-      <c r="E103" s="29"/>
-      <c r="F103" s="29"/>
+      <c r="E103" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F103" s="29" t="s">
+        <v>204</v>
+      </c>
       <c r="G103" s="7"/>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>

</xml_diff>

<commit_message>
Added AIP strategy tests
</commit_message>
<xml_diff>
--- a/4004-F18-A2-correctionGrid.xlsx
+++ b/4004-F18-A2-correctionGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thinkpad\Documents\GitHub\comp4004-A2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC2FB5-AA6C-4E3D-82AB-6EFD1841334C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF903BF1-4CEE-458F-9014-D650049E1C00}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="209">
   <si>
     <t>First Name</t>
   </si>
@@ -667,6 +667,12 @@
   </si>
   <si>
     <t>java file</t>
+  </si>
+  <si>
+    <t>AIP_exchanges.feature</t>
+  </si>
+  <si>
+    <t>AIPExchanges.java</t>
   </si>
 </sst>
 </file>
@@ -2208,8 +2214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A100" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4984,14 +4990,18 @@
         <v>111</v>
       </c>
       <c r="B105" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C105" s="23"/>
       <c r="D105" s="12">
         <v>1</v>
       </c>
-      <c r="E105" s="29"/>
-      <c r="F105" s="29"/>
+      <c r="E105" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F105" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G105" s="7"/>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
@@ -5008,14 +5018,18 @@
         <v>113</v>
       </c>
       <c r="B106" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C106" s="23"/>
       <c r="D106" s="12">
         <v>1</v>
       </c>
-      <c r="E106" s="29"/>
-      <c r="F106" s="29"/>
+      <c r="E106" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F106" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
@@ -5032,14 +5046,18 @@
         <v>112</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C107" s="23"/>
       <c r="D107" s="12">
         <v>1</v>
       </c>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
+      <c r="E107" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F107" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G107" s="7"/>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
@@ -5056,14 +5074,18 @@
         <v>114</v>
       </c>
       <c r="B108" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C108" s="23"/>
       <c r="D108" s="12">
         <v>1</v>
       </c>
-      <c r="E108" s="29"/>
-      <c r="F108" s="29"/>
+      <c r="E108" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F108" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G108" s="7"/>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
@@ -5080,14 +5102,18 @@
         <v>115</v>
       </c>
       <c r="B109" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C109" s="23"/>
       <c r="D109" s="12">
         <v>1</v>
       </c>
-      <c r="E109" s="29"/>
-      <c r="F109" s="29"/>
+      <c r="E109" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F109" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G109" s="7"/>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
@@ -5104,14 +5130,18 @@
         <v>116</v>
       </c>
       <c r="B110" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C110" s="23"/>
       <c r="D110" s="12">
         <v>1</v>
       </c>
-      <c r="E110" s="29"/>
-      <c r="F110" s="29"/>
+      <c r="E110" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F110" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G110" s="7"/>
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
@@ -5128,14 +5158,18 @@
         <v>117</v>
       </c>
       <c r="B111" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C111" s="23"/>
       <c r="D111" s="12">
         <v>1</v>
       </c>
-      <c r="E111" s="29"/>
-      <c r="F111" s="29"/>
+      <c r="E111" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F111" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G111" s="7"/>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
@@ -5152,14 +5186,18 @@
         <v>118</v>
       </c>
       <c r="B112" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C112" s="23"/>
       <c r="D112" s="12">
         <v>1</v>
       </c>
-      <c r="E112" s="29"/>
-      <c r="F112" s="29"/>
+      <c r="E112" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F112" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G112" s="7"/>
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
@@ -5176,14 +5214,18 @@
         <v>119</v>
       </c>
       <c r="B113" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C113" s="23"/>
       <c r="D113" s="12">
         <v>1</v>
       </c>
-      <c r="E113" s="29"/>
-      <c r="F113" s="29"/>
+      <c r="E113" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F113" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G113" s="7"/>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
@@ -5200,14 +5242,18 @@
         <v>120</v>
       </c>
       <c r="B114" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C114" s="23"/>
       <c r="D114" s="12">
         <v>1</v>
       </c>
-      <c r="E114" s="29"/>
-      <c r="F114" s="29"/>
+      <c r="E114" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F114" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G114" s="7"/>
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
@@ -5224,14 +5270,18 @@
         <v>121</v>
       </c>
       <c r="B115" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C115" s="23"/>
       <c r="D115" s="12">
         <v>1</v>
       </c>
-      <c r="E115" s="29"/>
-      <c r="F115" s="29"/>
+      <c r="E115" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F115" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G115" s="7"/>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
@@ -5248,14 +5298,18 @@
         <v>122</v>
       </c>
       <c r="B116" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C116" s="23"/>
       <c r="D116" s="12">
         <v>1</v>
       </c>
-      <c r="E116" s="29"/>
-      <c r="F116" s="29"/>
+      <c r="E116" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F116" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G116" s="7"/>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
@@ -5272,14 +5326,18 @@
         <v>123</v>
       </c>
       <c r="B117" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C117" s="23"/>
       <c r="D117" s="12">
         <v>1</v>
       </c>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
+      <c r="E117" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F117" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G117" s="7"/>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
@@ -5296,14 +5354,18 @@
         <v>124</v>
       </c>
       <c r="B118" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C118" s="23"/>
       <c r="D118" s="12">
         <v>1</v>
       </c>
-      <c r="E118" s="29"/>
-      <c r="F118" s="29"/>
+      <c r="E118" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F118" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G118" s="7"/>
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
@@ -5320,14 +5382,18 @@
         <v>125</v>
       </c>
       <c r="B119" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C119" s="23"/>
       <c r="D119" s="12">
         <v>1</v>
       </c>
-      <c r="E119" s="29"/>
-      <c r="F119" s="29"/>
+      <c r="E119" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F119" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G119" s="7"/>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
@@ -5344,14 +5410,18 @@
         <v>126</v>
       </c>
       <c r="B120" s="22" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C120" s="23"/>
       <c r="D120" s="12">
         <v>1</v>
       </c>
-      <c r="E120" s="29"/>
-      <c r="F120" s="29"/>
+      <c r="E120" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F120" s="29" t="s">
+        <v>208</v>
+      </c>
       <c r="G120" s="7"/>
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>

</xml_diff>